<commit_message>
Added color red style and Title tooltip
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/TodaysPlays stats.xlsx
+++ b/BballMVC/_Documentation/TodaysPlays stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1557EE-0754-4671-80EC-1F50D87DE120}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79261E97-F122-44E0-892C-E47E1CB91BC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="2400" windowWidth="28545" windowHeight="11835" activeTab="2" xr2:uid="{FC59E757-A7AC-4D2D-9ACF-0C6808134BA1}"/>
+    <workbookView xWindow="30030" yWindow="1785" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{FC59E757-A7AC-4D2D-9ACF-0C6808134BA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="75">
   <si>
     <t>GameDate</t>
   </si>
@@ -366,6 +366,24 @@
   </si>
   <si>
     <t>AverageMadeOpPt1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOU       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IND       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIL       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHO       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTA       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAC       </t>
   </si>
 </sst>
 </file>
@@ -461,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -471,6 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399F6080-8CE2-4D8D-934F-08F0BF20EF22}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection sqref="A1:Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,59 +825,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44235</v>
       </c>
@@ -912,7 +931,7 @@
       </c>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44236</v>
       </c>
@@ -966,7 +985,7 @@
       </c>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44236</v>
       </c>
@@ -1020,7 +1039,7 @@
       </c>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44238</v>
       </c>
@@ -1074,7 +1093,7 @@
       </c>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44239</v>
       </c>
@@ -1128,7 +1147,7 @@
       </c>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44239</v>
       </c>
@@ -1182,7 +1201,7 @@
       </c>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44239</v>
       </c>
@@ -1236,7 +1255,7 @@
       </c>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44239</v>
       </c>
@@ -1290,7 +1309,7 @@
       </c>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44239</v>
       </c>
@@ -1344,7 +1363,7 @@
       </c>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44239</v>
       </c>
@@ -1398,7 +1417,7 @@
       </c>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44240</v>
       </c>
@@ -1452,7 +1471,7 @@
       </c>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44241</v>
       </c>
@@ -1506,7 +1525,7 @@
       </c>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44241</v>
       </c>
@@ -1560,7 +1579,7 @@
       </c>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44241</v>
       </c>
@@ -1614,7 +1633,7 @@
       </c>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44241</v>
       </c>
@@ -1667,6 +1686,870 @@
         <v>101</v>
       </c>
       <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44242</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>521</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17">
+        <v>232</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="K17">
+        <v>1.01</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>250</v>
+      </c>
+      <c r="N17">
+        <v>-1</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>-100</v>
+      </c>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44242</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>531</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18">
+        <v>243</v>
+      </c>
+      <c r="I18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18">
+        <v>100</v>
+      </c>
+      <c r="K18">
+        <v>-1.08</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>261</v>
+      </c>
+      <c r="N18">
+        <v>-1</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>-108</v>
+      </c>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44243</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>537</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <v>230</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="K19">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>257</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>100</v>
+      </c>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44243</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>543</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20">
+        <v>225</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20">
+        <v>100</v>
+      </c>
+      <c r="K20">
+        <v>-1.05</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>219</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>100</v>
+      </c>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44244</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>551</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21">
+        <v>235</v>
+      </c>
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21">
+        <v>100</v>
+      </c>
+      <c r="K21">
+        <v>-1.06</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>258</v>
+      </c>
+      <c r="N21">
+        <v>-1</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>-106</v>
+      </c>
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>44244</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>555</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <v>228</v>
+      </c>
+      <c r="I22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="K22">
+        <v>-1.1499999999999999</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>231</v>
+      </c>
+      <c r="N22">
+        <v>-1</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>-115</v>
+      </c>
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>44244</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>561</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23">
+        <v>225</v>
+      </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23">
+        <v>100</v>
+      </c>
+      <c r="K23">
+        <v>-1.04</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>262</v>
+      </c>
+      <c r="N23">
+        <v>-1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>-104</v>
+      </c>
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>44246</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>509</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24">
+        <v>220</v>
+      </c>
+      <c r="I24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24">
+        <v>100</v>
+      </c>
+      <c r="K24">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>204</v>
+      </c>
+      <c r="N24">
+        <v>-1</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>-109</v>
+      </c>
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>44246</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>511</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25">
+        <v>232</v>
+      </c>
+      <c r="I25" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25">
+        <v>1.01</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>183</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>101</v>
+      </c>
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>44246</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>513</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <v>229</v>
+      </c>
+      <c r="I26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26">
+        <v>100</v>
+      </c>
+      <c r="K26">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>246</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>100</v>
+      </c>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>44246</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>519</v>
+      </c>
+      <c r="D27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27">
+        <v>224.5</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27">
+        <v>100</v>
+      </c>
+      <c r="K27">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>228</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>100</v>
+      </c>
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>44247</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <v>525</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28">
+        <v>223</v>
+      </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28">
+        <v>100</v>
+      </c>
+      <c r="K28">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>225</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>100</v>
+      </c>
+      <c r="R28" s="2"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>44247</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29">
+        <v>529</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29">
+        <v>236</v>
+      </c>
+      <c r="I29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29">
+        <v>100</v>
+      </c>
+      <c r="K29">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>236</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29" s="2"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>44247</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>531</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30">
+        <v>207.5</v>
+      </c>
+      <c r="I30" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30">
+        <v>100</v>
+      </c>
+      <c r="K30">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>190</v>
+      </c>
+      <c r="N30">
+        <v>-1</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>-110</v>
+      </c>
+      <c r="R30" s="2"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>44248</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>535</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31">
+        <v>230.5</v>
+      </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31">
+        <v>100</v>
+      </c>
+      <c r="K31">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31">
+        <v>235</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>100</v>
+      </c>
+      <c r="R31" s="2"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>44248</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>549</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32">
+        <v>238.5</v>
+      </c>
+      <c r="I32" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32">
+        <v>100</v>
+      </c>
+      <c r="K32">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>243</v>
+      </c>
+      <c r="N32">
+        <v>-1</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>-109</v>
+      </c>
+      <c r="R32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1675,10 +2558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01121B8B-CCBC-4137-A3DD-379BA7197A42}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,134 +2585,151 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <f t="shared" ref="A3:A8" si="0">A4+7</f>
-        <v>44241</v>
+        <f t="shared" ref="A3:A9" si="0">A4+7</f>
+        <v>44248</v>
       </c>
       <c r="B3">
-        <v>462</v>
+        <v>-160</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="1">C4+B3</f>
-        <v>-8848</v>
+        <f t="shared" ref="C3" si="1">C4+B3</f>
+        <v>-9008</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D8" si="2">D4+B3</f>
-        <v>317</v>
+        <f t="shared" ref="D3" si="2">D4+B3</f>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" si="0"/>
-        <v>44234</v>
+        <v>44241</v>
       </c>
       <c r="B4">
-        <v>67</v>
+        <v>462</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
-        <v>-9310</v>
+        <f t="shared" ref="C4:C10" si="3">C5+B4</f>
+        <v>-8848</v>
       </c>
       <c r="D4">
-        <f t="shared" si="2"/>
-        <v>-145</v>
+        <f t="shared" ref="D4:D9" si="4">D5+B4</f>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
-        <v>44227</v>
+        <v>44234</v>
       </c>
       <c r="B5">
-        <v>-887</v>
+        <v>67</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
-        <v>-9377</v>
+        <f t="shared" si="3"/>
+        <v>-9310</v>
       </c>
       <c r="D5">
-        <f t="shared" si="2"/>
-        <v>-212</v>
+        <f t="shared" si="4"/>
+        <v>-145</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
-        <v>44220</v>
+        <v>44227</v>
       </c>
       <c r="B6">
-        <v>264</v>
+        <v>-887</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
-        <v>-8490</v>
+        <f t="shared" si="3"/>
+        <v>-9377</v>
       </c>
       <c r="D6">
-        <f t="shared" si="2"/>
-        <v>675</v>
+        <f t="shared" si="4"/>
+        <v>-212</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
-        <v>44213</v>
+        <v>44220</v>
       </c>
       <c r="B7">
-        <v>369</v>
+        <v>264</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
-        <v>-8754</v>
+        <f t="shared" si="3"/>
+        <v>-8490</v>
       </c>
       <c r="D7">
-        <f t="shared" si="2"/>
-        <v>411</v>
+        <f t="shared" si="4"/>
+        <v>675</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
-        <v>44206</v>
+        <v>44213</v>
       </c>
       <c r="B8">
-        <v>-58</v>
+        <v>369</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>-9123</v>
+        <f t="shared" si="3"/>
+        <v>-8754</v>
       </c>
       <c r="D8">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="E8">
-        <v>151</v>
+        <f t="shared" si="4"/>
+        <v>411</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>44206</v>
+      </c>
+      <c r="B9">
+        <v>-58</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="3"/>
+        <v>-9123</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="E9">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>44199</v>
       </c>
-      <c r="B9">
-        <v>100</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="1"/>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="3"/>
         <v>-9065</v>
       </c>
-      <c r="D9">
-        <f>D10+B9</f>
-        <v>100</v>
-      </c>
-      <c r="E9">
+      <c r="D10">
+        <f>D11+B10</f>
+        <v>100</v>
+      </c>
+      <c r="E10">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="C10">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="C11">
         <v>-9165</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>83</v>
       </c>
     </row>
@@ -1843,7 +2743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A886D69D-7C55-49F4-8FC9-594458769A49}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated PGA. Before PGA switching lines 1 & 2
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/TodaysPlays stats.xlsx
+++ b/BballMVC/_Documentation/TodaysPlays stats.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79261E97-F122-44E0-892C-E47E1CB91BC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7E97D9-5A61-4347-BAA1-8EB5F4CAD614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30030" yWindow="1785" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{FC59E757-A7AC-4D2D-9ACF-0C6808134BA1}"/>
+    <workbookView xWindow="1335" yWindow="240" windowWidth="26160" windowHeight="13905" xr2:uid="{FC59E757-A7AC-4D2D-9ACF-0C6808134BA1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plays" sheetId="1" r:id="rId1"/>
     <sheet name="Weeklys" sheetId="2" r:id="rId2"/>
     <sheet name="TMs UI" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="72">
   <si>
     <t>GameDate</t>
   </si>
@@ -98,36 +98,21 @@
     <t xml:space="preserve">          </t>
   </si>
   <si>
-    <t xml:space="preserve">NY        </t>
-  </si>
-  <si>
     <t xml:space="preserve">MIA       </t>
   </si>
   <si>
     <t xml:space="preserve">Over      </t>
   </si>
   <si>
-    <t xml:space="preserve">PHI       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAC       </t>
-  </si>
-  <si>
     <t xml:space="preserve">TOR       </t>
   </si>
   <si>
     <t xml:space="preserve">BOS       </t>
   </si>
   <si>
-    <t xml:space="preserve">SA        </t>
-  </si>
-  <si>
     <t xml:space="preserve">ATL       </t>
   </si>
   <si>
-    <t xml:space="preserve">NO        </t>
-  </si>
-  <si>
     <t xml:space="preserve">DAL       </t>
   </si>
   <si>
@@ -137,19 +122,10 @@
     <t xml:space="preserve">DEN       </t>
   </si>
   <si>
-    <t xml:space="preserve">ORL       </t>
-  </si>
-  <si>
     <t xml:space="preserve">MEM       </t>
   </si>
   <si>
     <t xml:space="preserve">LAL       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DET       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BR        </t>
   </si>
   <si>
     <t xml:space="preserve">GS        </t>
@@ -385,12 +361,27 @@
   <si>
     <t xml:space="preserve">LAC       </t>
   </si>
+  <si>
+    <t xml:space="preserve">CHA       </t>
+  </si>
+  <si>
+    <t>Wins</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
+    <t>DailyResult</t>
+  </si>
+  <si>
+    <t>Dailys</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +407,13 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -479,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -490,6 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399F6080-8CE2-4D8D-934F-08F0BF20EF22}">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,30 +876,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44235</v>
+        <v>44249</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H2">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I2" t="s">
         <v>22</v>
@@ -909,52 +908,52 @@
         <v>100</v>
       </c>
       <c r="K2">
-        <v>-1.05</v>
+        <v>-1.1100000000000001</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <v>100</v>
+        <v>-111</v>
       </c>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44236</v>
+        <v>44249</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3">
-        <v>503</v>
+        <v>559</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="I3" t="s">
         <v>22</v>
@@ -963,43 +962,43 @@
         <v>100</v>
       </c>
       <c r="K3">
-        <v>-1.07</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="N3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>-107</v>
+        <v>100</v>
       </c>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>44236</v>
+        <v>44249</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4">
-        <v>509</v>
+        <v>563</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -1008,7 +1007,7 @@
         <v>21</v>
       </c>
       <c r="H4">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
@@ -1023,46 +1022,46 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>100</v>
+        <v>-108</v>
       </c>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>44238</v>
+        <v>44250</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5">
-        <v>221</v>
+        <v>223.5</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
@@ -1071,43 +1070,43 @@
         <v>100</v>
       </c>
       <c r="K5">
-        <v>-1.03</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>100</v>
+        <v>-110</v>
       </c>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>44239</v>
+        <v>44250</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6">
-        <v>545</v>
+        <v>577</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -1116,7 +1115,7 @@
         <v>21</v>
       </c>
       <c r="H6">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="I6" t="s">
         <v>22</v>
@@ -1125,13 +1124,13 @@
         <v>100</v>
       </c>
       <c r="K6">
-        <v>-1.0900000000000001</v>
+        <v>-1.03</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="N6">
         <v>-1</v>
@@ -1143,34 +1142,34 @@
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>-109</v>
+        <v>-103</v>
       </c>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>44239</v>
+        <v>44251</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7">
-        <v>549</v>
+        <v>501</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H7">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I7" t="s">
         <v>22</v>
@@ -1179,13 +1178,13 @@
         <v>100</v>
       </c>
       <c r="K7">
-        <v>-1.01</v>
+        <v>-1.07</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>273</v>
+        <v>218</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1201,30 +1200,30 @@
       </c>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>44239</v>
+        <v>44251</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>555</v>
+        <v>515</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H8">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="I8" t="s">
         <v>22</v>
@@ -1233,13 +1232,13 @@
         <v>100</v>
       </c>
       <c r="K8">
-        <v>-1.05</v>
+        <v>-1.07</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>192</v>
+        <v>245</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1255,30 +1254,30 @@
       </c>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>44239</v>
+        <v>44251</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9">
-        <v>557</v>
+        <v>517</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H9">
-        <v>223.5</v>
+        <v>218</v>
       </c>
       <c r="I9" t="s">
         <v>22</v>
@@ -1287,13 +1286,13 @@
         <v>100</v>
       </c>
       <c r="K9">
-        <v>-1.05</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="N9">
         <v>-1</v>
@@ -1305,34 +1304,34 @@
         <v>1</v>
       </c>
       <c r="Q9">
-        <v>-105</v>
+        <v>-110</v>
       </c>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>44239</v>
+        <v>44252</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10">
-        <v>559</v>
+        <v>525</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="I10" t="s">
         <v>22</v>
@@ -1341,52 +1340,52 @@
         <v>100</v>
       </c>
       <c r="K10">
-        <v>-1.05</v>
+        <v>-1.04</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <v>100</v>
+        <v>-104</v>
       </c>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>44239</v>
+        <v>44252</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11">
-        <v>575</v>
+        <v>527</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H11">
-        <v>211.5</v>
+        <v>238</v>
       </c>
       <c r="I11" t="s">
         <v>22</v>
@@ -1395,43 +1394,43 @@
         <v>100</v>
       </c>
       <c r="K11">
-        <v>-1.1000000000000001</v>
+        <v>-1.04</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="N11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>-110</v>
+        <v>100</v>
       </c>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>44240</v>
+        <v>44253</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12">
-        <v>569</v>
+        <v>535</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
@@ -1440,7 +1439,7 @@
         <v>21</v>
       </c>
       <c r="H12">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="I12" t="s">
         <v>22</v>
@@ -1449,13 +1448,13 @@
         <v>100</v>
       </c>
       <c r="K12">
-        <v>-1.08</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="N12">
         <v>-1</v>
@@ -1467,34 +1466,34 @@
         <v>1</v>
       </c>
       <c r="Q12">
-        <v>-108</v>
+        <v>-110</v>
       </c>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>44241</v>
+        <v>44253</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13">
-        <v>501</v>
+        <v>537</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13">
-        <v>234.5</v>
+        <v>225.5</v>
       </c>
       <c r="I13" t="s">
         <v>22</v>
@@ -1503,52 +1502,52 @@
         <v>100</v>
       </c>
       <c r="K13">
-        <v>-1.1100000000000001</v>
+        <v>-1.0900000000000001</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>239</v>
+        <v>203</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
-        <v>100</v>
+        <v>-109</v>
       </c>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>44241</v>
+        <v>44253</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
       <c r="C14">
-        <v>503</v>
+        <v>539</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H14">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
@@ -1557,43 +1556,43 @@
         <v>100</v>
       </c>
       <c r="K14">
-        <v>-1.06</v>
+        <v>-1.07</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>-107</v>
       </c>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>44241</v>
+        <v>44253</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
       </c>
       <c r="C15">
-        <v>577</v>
+        <v>543</v>
       </c>
       <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
         <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>18</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
@@ -1602,7 +1601,7 @@
         <v>21</v>
       </c>
       <c r="H15">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="I15" t="s">
         <v>22</v>
@@ -1611,52 +1610,52 @@
         <v>100</v>
       </c>
       <c r="K15">
-        <v>-1.05</v>
+        <v>-1.04</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>44241</v>
+        <v>44253</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16">
-        <v>579</v>
+        <v>547</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H16">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="I16" t="s">
         <v>22</v>
@@ -1665,40 +1664,40 @@
         <v>100</v>
       </c>
       <c r="K16">
-        <v>1.01</v>
+        <v>-1.0900000000000001</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16">
-        <v>101</v>
+        <v>-109</v>
       </c>
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>44242</v>
+        <v>44254</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
-        <v>521</v>
+        <v>555</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
@@ -1710,7 +1709,7 @@
         <v>21</v>
       </c>
       <c r="H17">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="I17" t="s">
         <v>22</v>
@@ -1719,13 +1718,13 @@
         <v>100</v>
       </c>
       <c r="K17">
-        <v>1.01</v>
+        <v>-1.06</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="N17">
         <v>-1</v>
@@ -1737,34 +1736,34 @@
         <v>1</v>
       </c>
       <c r="Q17">
-        <v>-100</v>
+        <v>-106</v>
       </c>
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>44242</v>
+        <v>44255</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18">
-        <v>531</v>
+        <v>563</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H18">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="I18" t="s">
         <v>22</v>
@@ -1773,13 +1772,13 @@
         <v>100</v>
       </c>
       <c r="K18">
-        <v>-1.08</v>
+        <v>-1.05</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>261</v>
+        <v>205</v>
       </c>
       <c r="N18">
         <v>-1</v>
@@ -1791,34 +1790,34 @@
         <v>1</v>
       </c>
       <c r="Q18">
-        <v>-108</v>
+        <v>-105</v>
       </c>
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>44243</v>
+        <v>44255</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19">
-        <v>537</v>
+        <v>569</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="F19" t="s">
         <v>20</v>
       </c>
       <c r="G19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H19">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="I19" t="s">
         <v>22</v>
@@ -1827,43 +1826,43 @@
         <v>100</v>
       </c>
       <c r="K19">
-        <v>-1.1000000000000001</v>
+        <v>-1.05</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="N19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19">
-        <v>100</v>
+        <v>-105</v>
       </c>
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44243</v>
+        <v>44255</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20">
-        <v>543</v>
+        <v>575</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
         <v>20</v>
@@ -1881,13 +1880,13 @@
         <v>100</v>
       </c>
       <c r="K20">
-        <v>-1.05</v>
+        <v>-1.08</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -1903,656 +1902,132 @@
       </c>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>44244</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21">
-        <v>551</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21">
-        <v>235</v>
-      </c>
-      <c r="I21" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21">
-        <v>100</v>
-      </c>
-      <c r="K21">
-        <v>-1.06</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>258</v>
-      </c>
-      <c r="N21">
-        <v>-1</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-      <c r="Q21">
-        <v>-106</v>
-      </c>
-      <c r="R21" s="2"/>
+    <row r="21" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Q21" s="10">
+        <f>SUM(Q2:Q20)</f>
+        <v>-897</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>44244</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22">
-        <v>555</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22">
-        <v>228</v>
-      </c>
-      <c r="I22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22">
-        <v>100</v>
-      </c>
-      <c r="K22">
-        <v>-1.1499999999999999</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>231</v>
-      </c>
-      <c r="N22">
-        <v>-1</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>1</v>
-      </c>
-      <c r="Q22">
-        <v>-115</v>
-      </c>
-      <c r="R22" s="2"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>44244</v>
-      </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23">
-        <v>561</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="D23" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23">
-        <v>225</v>
-      </c>
-      <c r="I23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23">
-        <v>100</v>
-      </c>
-      <c r="K23">
-        <v>-1.04</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>262</v>
-      </c>
-      <c r="N23">
-        <v>-1</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>1</v>
-      </c>
-      <c r="Q23">
-        <v>-104</v>
-      </c>
-      <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>44246</v>
-      </c>
-      <c r="B24" t="s">
-        <v>17</v>
+        <v>44249</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>509</v>
-      </c>
-      <c r="D24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24">
-        <v>220</v>
-      </c>
-      <c r="I24" t="s">
-        <v>22</v>
-      </c>
-      <c r="J24">
-        <v>100</v>
-      </c>
-      <c r="K24">
-        <v>-1.0900000000000001</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>204</v>
-      </c>
-      <c r="N24">
-        <v>-1</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>1</v>
-      </c>
-      <c r="Q24">
-        <v>-109</v>
-      </c>
-      <c r="R24" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>-119</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>44246</v>
-      </c>
-      <c r="B25" t="s">
-        <v>17</v>
+        <v>44250</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>511</v>
-      </c>
-      <c r="D25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25">
-        <v>232</v>
-      </c>
-      <c r="I25" t="s">
-        <v>22</v>
-      </c>
-      <c r="J25">
-        <v>100</v>
-      </c>
-      <c r="K25">
-        <v>1.01</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>183</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <v>101</v>
-      </c>
-      <c r="R25" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>-213</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>44246</v>
-      </c>
-      <c r="B26" t="s">
-        <v>17</v>
+        <v>44251</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>513</v>
-      </c>
-      <c r="D26" t="s">
-        <v>72</v>
-      </c>
-      <c r="E26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26">
-        <v>229</v>
-      </c>
-      <c r="I26" t="s">
-        <v>22</v>
-      </c>
-      <c r="J26">
-        <v>100</v>
-      </c>
-      <c r="K26">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>246</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>100</v>
-      </c>
-      <c r="R26" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>90</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>44246</v>
-      </c>
-      <c r="B27" t="s">
-        <v>17</v>
+        <v>44252</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>519</v>
-      </c>
-      <c r="D27" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27">
-        <v>224.5</v>
-      </c>
-      <c r="I27" t="s">
-        <v>22</v>
-      </c>
-      <c r="J27">
-        <v>100</v>
-      </c>
-      <c r="K27">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>228</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="O27">
-        <v>1</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>100</v>
-      </c>
-      <c r="R27" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>-4</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>44247</v>
-      </c>
-      <c r="B28" t="s">
-        <v>17</v>
+        <v>44253</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>525</v>
-      </c>
-      <c r="D28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28">
-        <v>223</v>
-      </c>
-      <c r="I28" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28">
-        <v>100</v>
-      </c>
-      <c r="K28">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>225</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
-      <c r="O28">
-        <v>1</v>
-      </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <v>100</v>
-      </c>
-      <c r="R28" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>-435</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>44247</v>
-      </c>
-      <c r="B29" t="s">
-        <v>17</v>
+        <v>44254</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>529</v>
-      </c>
-      <c r="D29" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29">
-        <v>236</v>
-      </c>
-      <c r="I29" t="s">
-        <v>22</v>
-      </c>
-      <c r="J29">
-        <v>100</v>
-      </c>
-      <c r="K29">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>236</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>-106</v>
+      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>44247</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
+        <v>44255</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>531</v>
-      </c>
-      <c r="D30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30">
-        <v>207.5</v>
-      </c>
-      <c r="I30" t="s">
-        <v>22</v>
-      </c>
-      <c r="J30">
-        <v>100</v>
-      </c>
-      <c r="K30">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>190</v>
-      </c>
-      <c r="N30">
-        <v>-1</v>
-      </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-      <c r="P30">
-        <v>1</v>
-      </c>
-      <c r="Q30">
+        <v>2</v>
+      </c>
+      <c r="D30">
         <v>-110</v>
       </c>
-      <c r="R30" s="2"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>44248</v>
-      </c>
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31">
-        <v>535</v>
-      </c>
-      <c r="D31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31">
-        <v>230.5</v>
-      </c>
-      <c r="I31" t="s">
-        <v>22</v>
-      </c>
-      <c r="J31">
-        <v>100</v>
-      </c>
-      <c r="K31">
-        <v>-1.0900000000000001</v>
-      </c>
-      <c r="L31">
-        <v>2</v>
-      </c>
-      <c r="M31">
-        <v>235</v>
-      </c>
-      <c r="N31">
-        <v>1</v>
-      </c>
-      <c r="O31">
-        <v>1</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>100</v>
-      </c>
-      <c r="R31" s="2"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>44248</v>
-      </c>
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32">
-        <v>549</v>
-      </c>
-      <c r="D32" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" t="s">
-        <v>71</v>
-      </c>
-      <c r="F32" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32">
-        <v>238.5</v>
-      </c>
-      <c r="I32" t="s">
-        <v>22</v>
-      </c>
-      <c r="J32">
-        <v>100</v>
-      </c>
-      <c r="K32">
-        <v>-1.0900000000000001</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32">
-        <v>243</v>
-      </c>
-      <c r="N32">
-        <v>-1</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-      <c r="P32">
-        <v>1</v>
-      </c>
-      <c r="Q32">
-        <v>-109</v>
-      </c>
-      <c r="R32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2560,7 +2035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01121B8B-CCBC-4137-A3DD-379BA7197A42}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -2571,16 +2046,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2761,92 +2236,92 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>13.1</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>5.0999999999999996</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>3.3</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>